<commit_message>
- Added new DecimalPlaces property for ClassToExcelRowAttribute - ClassToExcelRowConverter will now write to private properties.
</commit_message>
<xml_diff>
--- a/src/ClassToExcel.Sample.Data/Beverages.xlsx
+++ b/src/ClassToExcel.Sample.Data/Beverages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Beverages</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Avg. Number of Liters</t>
   </si>
 </sst>
 </file>
@@ -131,12 +137,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Beverages"/>
     <tableColumn id="2" name="Column1"/>
     <tableColumn id="3" name="Quantity"/>
+    <tableColumn id="4" name="Price"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -439,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +459,7 @@
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,48 +469,74 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2.1539999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>10.257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -514,7 +547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -525,7 +558,7 @@
         <v>41896</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>

</xml_diff>